<commit_message>
Add some files into gitignore to avoid conflict
</commit_message>
<xml_diff>
--- a/Document/Design-Entities-In-More-Detail.xlsx
+++ b/Document/Design-Entities-In-More-Detail.xlsx
@@ -5,15 +5,28 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-Book-Store-Website-Project\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PTIT-BookStore-Website-Project\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5939BA78-34BF-4473-A2E7-3A686DED1AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ABAB4B-DDCB-442A-809B-B90E8B9653C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Book" sheetId="1" r:id="rId1"/>
+    <sheet name="QuickLook" sheetId="20" r:id="rId1"/>
+    <sheet name="Book" sheetId="1" r:id="rId2"/>
+    <sheet name="Category" sheetId="2" r:id="rId3"/>
+    <sheet name="Publisher" sheetId="3" r:id="rId4"/>
+    <sheet name="Account" sheetId="9" r:id="rId5"/>
+    <sheet name="OrderDetail" sheetId="7" r:id="rId6"/>
+    <sheet name="Order" sheetId="6" r:id="rId7"/>
+    <sheet name="Role" sheetId="11" r:id="rId8"/>
+    <sheet name="WebAction" sheetId="17" r:id="rId9"/>
+    <sheet name="ActionRole" sheetId="18" r:id="rId10"/>
+    <sheet name="ShoppingCart" sheetId="13" r:id="rId11"/>
+    <sheet name="HistoryTable" sheetId="15" r:id="rId12"/>
+    <sheet name="SatisfyProduct" sheetId="14" r:id="rId13"/>
+    <sheet name="Rating" sheetId="16" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -69,15 +82,9 @@
     <t>Tác giả</t>
   </si>
   <si>
-    <t>char(6)</t>
-  </si>
-  <si>
     <t>Năm xuất bản</t>
   </si>
   <si>
-    <t>int(10)</t>
-  </si>
-  <si>
     <t>NOT NULL, DEFAULT= 0</t>
   </si>
   <si>
@@ -153,9 +160,6 @@
     <t>Discount%</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
     <t>Có đang giảm giá không</t>
   </si>
   <si>
@@ -163,13 +167,283 @@
   </si>
   <si>
     <t>Publisher</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>PublisherID</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>FK, NOT NULL</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>Mã thể loại</t>
+  </si>
+  <si>
+    <t>Tên thể loại</t>
+  </si>
+  <si>
+    <t>Tên nhà xuất bản</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn bán</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>Giờ lập</t>
+  </si>
+  <si>
+    <t>Tổng tiền</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>nvarchar(50)</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>TotalPrice</t>
+  </si>
+  <si>
+    <t>CustomerID</t>
+  </si>
+  <si>
+    <t>Số lượng, &lt; 127 (nếu muốn mua nhiều thì contact với store để tránh tình trạng boom hàng lớn)</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Mật khẩu, sẽ được mã hóa bằng jasypt</t>
+  </si>
+  <si>
+    <t>PK, NOT NULL</t>
+  </si>
+  <si>
+    <t>Mã quyền</t>
+  </si>
+  <si>
+    <t>Tên quyền</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>RoleID</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Actived</t>
+  </si>
+  <si>
+    <t>Trạng thái: 0 là chưa kích hoạt, 1 là đã kích hoạt</t>
+  </si>
+  <si>
+    <t>NOT NULL, UNIQUE</t>
+  </si>
+  <si>
+    <t>PK, NOT NULL, ID tăng dần</t>
+  </si>
+  <si>
+    <t>WebAction</t>
+  </si>
+  <si>
+    <t>Action ID</t>
+  </si>
+  <si>
+    <t>Tên của hành động</t>
+  </si>
+  <si>
+    <t>Mô tả hành động này được làm gì</t>
+  </si>
+  <si>
+    <t>ActionRole</t>
+  </si>
+  <si>
+    <t>ActionID</t>
+  </si>
+  <si>
+    <t>CustomerAddress</t>
+  </si>
+  <si>
+    <t>CustomerPhone</t>
+  </si>
+  <si>
+    <t>Địa chỉ nhận hàng</t>
+  </si>
+  <si>
+    <t>SĐT người nhận</t>
+  </si>
+  <si>
+    <t>ConsigneeAddress</t>
+  </si>
+  <si>
+    <t>ConsigneePhone</t>
+  </si>
+  <si>
+    <t>ConsigneeName</t>
+  </si>
+  <si>
+    <t>Tên người nhận</t>
+  </si>
+  <si>
+    <t>Ngày đặt</t>
+  </si>
+  <si>
+    <t>ShoppingCart</t>
+  </si>
+  <si>
+    <t>&lt; 127</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>Mã sách</t>
+  </si>
+  <si>
+    <t>SatisfyProduct</t>
+  </si>
+  <si>
+    <t>HistoryID</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>RequestTime</t>
+  </si>
+  <si>
+    <t>SessionID</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>Mã lịch sử</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>OrderDetail</t>
+  </si>
+  <si>
+    <t>NOT NULL, ID tăng dần</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>BOOK</t>
+  </si>
+  <si>
+    <t>Pwd</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>URLImage</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>CustomerUsername</t>
+  </si>
+  <si>
+    <t>CustomerEmail</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>OrderID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +464,40 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,8 +516,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -234,21 +552,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,11 +986,734 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31671EE4-8A70-4D66-8D30-4AF13BB185ED}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="28"/>
+    <col min="3" max="3" width="17" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="28"/>
+    <col min="5" max="5" width="17" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="28"/>
+    <col min="7" max="7" width="11.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="28"/>
+    <col min="9" max="9" width="9.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="28"/>
+    <col min="11" max="11" width="11.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G12" s="31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CF813F-9AC6-4C19-9F1F-99EB074D6DC5}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96509950-CAC0-4D90-ABD8-6E056E488860}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4521A51E-E4F8-460B-8C55-1BD36CEA7242}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF6A5207-20FB-45F6-B362-A8348B15A2E8}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F09ABAE-B1A9-4FD3-A2CF-DFA89FDCB5E3}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="16"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,13 +1726,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -572,14 +1753,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
@@ -589,7 +1768,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -606,16 +1785,14 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>12</v>
@@ -623,7 +1800,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -640,19 +1817,17 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,145 +1835,908 @@
         <v>45</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEDA87D-BAC4-4352-B9B7-F62EB4492B9B}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A69C1AB7-BD7B-4572-9F9A-2F793DE53279}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="2" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19">
-        <v>300</v>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB03620-C75E-4C6E-9A95-CF8E4A2E7759}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C2A44DA-A465-4E76-9BE9-188B86B647BC}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D3:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDB18D0-D382-4879-8C95-88FA2EFB4320}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A37F61-B24F-45FD-B063-7F9E5EE7B923}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD3FF30F-D12C-41BF-B0F7-FAAC96004E3D}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="13"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>